<commit_message>
Cleaned up code and naming convention Edited default_animal_config.xlsx to change all n/a to 0. Code now works for all animal types
</commit_message>
<xml_diff>
--- a/default_configs/default_animal_config.xlsx
+++ b/default_configs/default_animal_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achermann\Project ReFuel\LCA tool developement\Manure Tool\default_configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBE07FD-7380-4494-BD21-DCE53A40351C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFB5E94-0322-4BB9-A018-2AE0D4444D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57435" yWindow="-165" windowWidth="29130" windowHeight="17610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="1185" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="58">
   <si>
     <t>kg/y</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Unit manure</t>
-  </si>
-  <si>
-    <t>n/a</t>
   </si>
   <si>
     <t>NL/kg odw</t>
@@ -554,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -593,105 +590,105 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>34</v>
-      </c>
-      <c r="I1" t="s">
-        <v>35</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
       </c>
       <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>37</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>38</v>
-      </c>
-      <c r="N1" t="s">
-        <v>39</v>
       </c>
       <c r="O1" t="s">
         <v>1</v>
       </c>
       <c r="P1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" t="s">
         <v>41</v>
       </c>
-      <c r="R1" t="s">
-        <v>54</v>
-      </c>
-      <c r="S1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T1" t="s">
-        <v>53</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>42</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>43</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>44</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>45</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>47</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" t="s">
-        <v>51</v>
-      </c>
       <c r="AE1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -727,14 +724,14 @@
         <v>14</v>
       </c>
       <c r="O2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P2">
         <v>270</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S2">
         <v>0.77900000000000003</v>
@@ -772,10 +769,10 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -805,14 +802,14 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P3">
         <v>270</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S3">
         <v>0.77900000000000003</v>
@@ -850,10 +847,10 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -886,14 +883,14 @@
         <v>14</v>
       </c>
       <c r="O4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P4">
         <v>270</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S4">
         <v>0.77900000000000003</v>
@@ -931,10 +928,10 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -964,14 +961,14 @@
         <v>14</v>
       </c>
       <c r="O5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P5">
         <v>270</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S5">
         <v>0.77900000000000003</v>
@@ -1009,10 +1006,10 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1042,14 +1039,14 @@
         <v>14</v>
       </c>
       <c r="O6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P6">
         <v>270</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S6">
         <v>0.77900000000000003</v>
@@ -1087,10 +1084,10 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1120,14 +1117,14 @@
         <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P7">
         <v>270</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S7">
         <v>0.77900000000000003</v>
@@ -1165,10 +1162,10 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1198,14 +1195,14 @@
         <v>14</v>
       </c>
       <c r="O8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P8">
         <v>270</v>
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S8">
         <v>0.77900000000000003</v>
@@ -1243,10 +1240,10 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1276,14 +1273,14 @@
         <v>14</v>
       </c>
       <c r="O9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P9">
         <v>270</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S9">
         <v>0.77900000000000003</v>
@@ -1321,10 +1318,10 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1354,14 +1351,14 @@
         <v>14</v>
       </c>
       <c r="O10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P10">
         <v>270</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S10">
         <v>0.77900000000000003</v>
@@ -1399,10 +1396,10 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1432,14 +1429,14 @@
         <v>14</v>
       </c>
       <c r="O11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P11">
         <v>270</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S11">
         <v>0.77900000000000003</v>
@@ -1477,10 +1474,10 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1510,14 +1507,14 @@
         <v>14</v>
       </c>
       <c r="O12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P12">
         <v>270</v>
       </c>
       <c r="Q12" s="1"/>
       <c r="R12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S12">
         <v>0.77900000000000003</v>
@@ -1555,10 +1552,10 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1588,14 +1585,14 @@
         <v>14</v>
       </c>
       <c r="O13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P13">
         <v>270</v>
       </c>
       <c r="Q13" s="1"/>
       <c r="R13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S13">
         <v>0.77900000000000003</v>
@@ -1633,10 +1630,10 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1666,14 +1663,14 @@
         <v>14</v>
       </c>
       <c r="O14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P14">
         <v>270</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S14">
         <v>0.77900000000000003</v>
@@ -1711,10 +1708,10 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1744,14 +1741,14 @@
         <v>14</v>
       </c>
       <c r="O15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P15">
         <v>270</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S15">
         <v>0.77900000000000003</v>
@@ -1789,10 +1786,10 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1822,14 +1819,14 @@
         <v>14</v>
       </c>
       <c r="O16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P16">
         <v>270</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="R16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S16">
         <v>0.77900000000000003</v>
@@ -1867,10 +1864,10 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1900,14 +1897,14 @@
         <v>14</v>
       </c>
       <c r="O17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P17">
         <v>270</v>
       </c>
       <c r="Q17" s="1"/>
       <c r="R17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S17">
         <v>0.77900000000000003</v>
@@ -1945,10 +1942,10 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1978,14 +1975,14 @@
         <v>14</v>
       </c>
       <c r="O18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P18">
         <v>270</v>
       </c>
       <c r="Q18" s="1"/>
       <c r="R18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S18">
         <v>0.77900000000000003</v>
@@ -2023,10 +2020,10 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -2056,14 +2053,14 @@
         <v>14</v>
       </c>
       <c r="O19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P19">
         <v>270</v>
       </c>
       <c r="Q19" s="1"/>
       <c r="R19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S19">
         <v>0.77900000000000003</v>
@@ -2101,10 +2098,10 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2134,14 +2131,14 @@
         <v>14</v>
       </c>
       <c r="O20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P20">
         <v>270</v>
       </c>
       <c r="Q20" s="1"/>
       <c r="R20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S20">
         <v>0.77900000000000003</v>
@@ -2179,10 +2176,10 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2212,14 +2209,14 @@
         <v>14</v>
       </c>
       <c r="O21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P21">
         <v>270</v>
       </c>
       <c r="Q21" s="1"/>
       <c r="R21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S21">
         <v>0.77900000000000003</v>
@@ -2257,10 +2254,10 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -2290,14 +2287,14 @@
         <v>14</v>
       </c>
       <c r="O22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P22">
         <v>270</v>
       </c>
       <c r="Q22" s="1"/>
       <c r="R22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S22">
         <v>0.77900000000000003</v>
@@ -2335,10 +2332,10 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2361,16 +2358,22 @@
       <c r="L23">
         <v>3</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
         <v>3</v>
-      </c>
-      <c r="O23" t="s">
-        <v>4</v>
       </c>
       <c r="P23">
         <v>270</v>
       </c>
       <c r="Q23" s="1"/>
+      <c r="R23" t="s">
+        <v>54</v>
+      </c>
       <c r="S23">
         <v>0.77900000000000003</v>
       </c>
@@ -2386,11 +2389,17 @@
       <c r="X23">
         <v>0.02</v>
       </c>
-      <c r="Y23" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>3</v>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
       </c>
       <c r="AC23">
         <v>3.9</v>
@@ -2401,10 +2410,10 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2427,16 +2436,22 @@
       <c r="L24">
         <v>3</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
         <v>3</v>
-      </c>
-      <c r="O24" t="s">
-        <v>4</v>
       </c>
       <c r="P24">
         <v>270</v>
       </c>
       <c r="Q24" s="1"/>
+      <c r="R24" t="s">
+        <v>54</v>
+      </c>
       <c r="S24">
         <v>0.77900000000000003</v>
       </c>
@@ -2452,11 +2467,17 @@
       <c r="X24">
         <v>0.02</v>
       </c>
-      <c r="Y24" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>3</v>
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+      <c r="AB24">
+        <v>0</v>
       </c>
       <c r="AC24">
         <v>44</v>
@@ -2467,10 +2488,10 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -2487,8 +2508,11 @@
       <c r="J25" t="s">
         <v>0</v>
       </c>
-      <c r="K25" t="s">
-        <v>3</v>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
       </c>
       <c r="M25">
         <v>259</v>
@@ -2497,20 +2521,29 @@
         <v>9</v>
       </c>
       <c r="O25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P25">
         <v>270</v>
       </c>
       <c r="Q25" s="1"/>
+      <c r="R25" t="s">
+        <v>54</v>
+      </c>
       <c r="S25">
         <v>0.77900000000000003</v>
       </c>
-      <c r="U25" t="s">
-        <v>3</v>
-      </c>
-      <c r="W25" t="s">
-        <v>3</v>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
       </c>
       <c r="Y25">
         <v>0.53</v>
@@ -2533,10 +2566,10 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -2553,8 +2586,11 @@
       <c r="J26" t="s">
         <v>0</v>
       </c>
-      <c r="K26" t="s">
-        <v>3</v>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
       </c>
       <c r="M26">
         <v>259</v>
@@ -2563,20 +2599,29 @@
         <v>9</v>
       </c>
       <c r="O26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P26">
         <v>270</v>
       </c>
       <c r="Q26" s="1"/>
+      <c r="R26" t="s">
+        <v>54</v>
+      </c>
       <c r="S26">
         <v>0.77900000000000003</v>
       </c>
-      <c r="U26" t="s">
-        <v>3</v>
-      </c>
-      <c r="W26" t="s">
-        <v>3</v>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
       </c>
       <c r="Y26">
         <v>0.53</v>
@@ -2599,10 +2644,10 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -2619,8 +2664,11 @@
       <c r="J27" t="s">
         <v>0</v>
       </c>
-      <c r="K27" t="s">
-        <v>3</v>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
       </c>
       <c r="M27">
         <v>259</v>
@@ -2629,20 +2677,29 @@
         <v>9</v>
       </c>
       <c r="O27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P27">
         <v>270</v>
       </c>
       <c r="Q27" s="1"/>
+      <c r="R27" t="s">
+        <v>54</v>
+      </c>
       <c r="S27">
         <v>0.77900000000000003</v>
       </c>
-      <c r="U27" t="s">
-        <v>3</v>
-      </c>
-      <c r="W27" t="s">
-        <v>3</v>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
       </c>
       <c r="Y27">
         <v>0.53</v>

</xml_diff>